<commit_message>
Add sql report sequece
</commit_message>
<xml_diff>
--- a/data_elec/abet-so-criterios-asignaturas.xlsx
+++ b/data_elec/abet-so-criterios-asignaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablo/Documents/dev/UPS/ABET/back/db/data_elec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EF1BD3-EB32-8A4D-8299-B4A0D172EA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C446D7-4689-6048-87EF-7A2E3C3F5AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25360" windowHeight="18880" activeTab="1" xr2:uid="{E56F2DA0-A1A5-9641-94A5-C6E94DEB89E6}"/>
   </bookViews>
@@ -898,7 +898,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -914,8 +914,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFAE81FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -926,6 +939,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1012,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1056,6 +1075,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2136,10 +2157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF80253E-E859-BC4A-9C77-1036EFC970CA}">
-  <dimension ref="A2:T55"/>
+  <dimension ref="A2:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3917,7 +3938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3976,7 +3997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3998,44 +4019,44 @@
       <c r="G50">
         <v>3</v>
       </c>
-      <c r="H50">
+      <c r="J50">
         <v>8</v>
       </c>
-      <c r="I50">
+      <c r="K50">
         <v>9</v>
       </c>
-      <c r="J50">
+      <c r="L50">
         <v>11</v>
       </c>
-      <c r="K50">
+      <c r="M50">
         <v>12</v>
       </c>
-      <c r="L50">
+      <c r="N50">
         <v>14</v>
       </c>
-      <c r="M50">
+      <c r="O50">
         <v>15</v>
       </c>
-      <c r="N50">
+      <c r="P50">
         <v>17</v>
       </c>
-      <c r="O50">
+      <c r="Q50">
         <v>18</v>
       </c>
-      <c r="P50">
+      <c r="R50">
         <v>19</v>
       </c>
-      <c r="Q50">
+      <c r="S50">
         <v>20</v>
       </c>
-      <c r="R50">
+      <c r="T50">
         <v>22</v>
       </c>
-      <c r="S50">
+      <c r="U50">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4070,7 +4091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4105,10 +4126,81 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E53" s="15">
+        <v>1</v>
+      </c>
+      <c r="F53" s="15">
+        <v>2</v>
+      </c>
+      <c r="G53" s="15">
+        <v>3</v>
+      </c>
+      <c r="H53" s="15">
+        <v>5</v>
+      </c>
+      <c r="I53" s="15">
+        <v>6</v>
+      </c>
+      <c r="J53" s="15">
+        <v>8</v>
+      </c>
+      <c r="K53" s="15">
+        <v>9</v>
+      </c>
+      <c r="L53" s="15">
+        <v>11</v>
+      </c>
+      <c r="M53" s="15">
+        <v>12</v>
+      </c>
+      <c r="N53" s="15">
+        <v>14</v>
+      </c>
+      <c r="O53" s="15">
+        <v>15</v>
+      </c>
+      <c r="P53" s="15">
+        <v>17</v>
+      </c>
+      <c r="Q53" s="15">
+        <v>18</v>
+      </c>
+      <c r="R53" s="15">
+        <v>19</v>
+      </c>
+      <c r="S53" s="15">
+        <v>20</v>
+      </c>
+      <c r="T53" s="15">
+        <v>22</v>
+      </c>
+      <c r="U53" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T55">
         <f>SUM(T3:T52)</f>
-        <v>274</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q56" s="16">
+        <v>328</v>
+      </c>
+      <c r="R56">
+        <v>17</v>
+      </c>
+      <c r="S56">
+        <f>Q56+R56</f>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S57">
+        <f>S56+R56</f>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>